<commit_message>
Update Risk Management-Added Substitute Risks
</commit_message>
<xml_diff>
--- a/Project Documents/Risk Management.xlsx
+++ b/Project Documents/Risk Management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael Chung\MITRE\MITR-RCC-Project\Project Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3B2D685-0345-4055-B853-A299794EBB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7DAF8B4-770E-4EE7-9E30-587C2AF2EABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Risk Category</t>
   </si>
@@ -114,6 +114,39 @@
 6. Insert the answer to question 5 into this spreadsheet in cell A16 with red font color.
 7. Submit this "Risk Managment In-Class Exercise" Spreadsheet with a file name that begins with your last name and the Edited "Risk Analysis" Spreadsheet with a file name that begins with your last name on LMS.
 </t>
+  </si>
+  <si>
+    <t>Technical Challenges</t>
+  </si>
+  <si>
+    <t>Cybersecurity threats</t>
+  </si>
+  <si>
+    <t>Lack of User Adoption</t>
+  </si>
+  <si>
+    <t>Data Security</t>
+  </si>
+  <si>
+    <t>Change in Requirements</t>
+  </si>
+  <si>
+    <t>Integration faults</t>
+  </si>
+  <si>
+    <t>Data Integrity</t>
+  </si>
+  <si>
+    <t>Scope Creep</t>
+  </si>
+  <si>
+    <t>Regulatory compliance</t>
+  </si>
+  <si>
+    <t>Client/Organization Approval</t>
+  </si>
+  <si>
+    <t>Third Party Approval</t>
   </si>
 </sst>
 </file>
@@ -448,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -821,18 +854,65 @@
         <v>-18205</v>
       </c>
     </row>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="2:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>